<commit_message>
feat(xlspython): write multidelcols to delete columns on multiple files
</commit_message>
<xml_diff>
--- a/fichiers_xls/gathertests/Nouveau dossier - Copie/test_keep_only_columns.xlsx
+++ b/fichiers_xls/gathertests/Nouveau dossier - Copie/test_keep_only_columns.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="9">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -40,21 +40,6 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <color rgb="FF969696"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="FFFF00FF"/>
       <sz val="10"/>
     </font>
     <font>
@@ -121,7 +106,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -129,12 +114,6 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -146,17 +125,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -166,6 +136,9 @@
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -275,8 +248,8 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.305081579275128"/>
-          <y val="0.0279194288628251"/>
+          <x val="0.305100579186648"/>
+          <y val="0.0280504908835905"/>
         </manualLayout>
       </layout>
       <overlay val="0"/>
@@ -295,10 +268,10 @@
           <yMode val="edge"/>
           <wMode val="factor"/>
           <hMode val="factor"/>
-          <x val="0.0127039481878192"/>
-          <y val="0.125318714941356"/>
-          <w val="0.964628222692739"/>
-          <h val="0.858618052014278"/>
+          <x val="0.0127047393660086"/>
+          <y val="0.125334693357134"/>
+          <w val="0.9645637416703"/>
+          <h val="0.858472523269157"/>
         </manualLayout>
       </layout>
       <barChart>
@@ -471,11 +444,11 @@
         </ser>
         <gapWidth val="219"/>
         <overlap val="-27"/>
-        <axId val="60289730"/>
-        <axId val="26290805"/>
+        <axId val="97293934"/>
+        <axId val="54435663"/>
       </barChart>
       <catAx>
-        <axId val="60289730"/>
+        <axId val="97293934"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
@@ -510,7 +483,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="26290805"/>
+        <crossAx val="54435663"/>
         <crossesAt val="0"/>
         <auto val="1"/>
         <lblAlgn val="ctr"/>
@@ -518,7 +491,7 @@
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="26290805"/>
+        <axId val="54435663"/>
         <scaling>
           <orientation val="minMax"/>
           <max val="100"/>
@@ -562,7 +535,7 @@
             </a:r>
           </a:p>
         </txPr>
-        <crossAx val="60289730"/>
+        <crossAx val="97293934"/>
         <crossesAt val="1"/>
         <crossBetween val="midCat"/>
       </valAx>
@@ -588,16 +561,16 @@
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor editAs="oneCell">
     <from>
-      <col>99</col>
-      <colOff>10080</colOff>
-      <row>13</row>
-      <rowOff>93960</rowOff>
+      <col>128</col>
+      <colOff>504000</colOff>
+      <row>16</row>
+      <rowOff>103320</rowOff>
     </from>
     <to>
-      <col>106</col>
-      <colOff>34200</colOff>
-      <row>30</row>
-      <rowOff>126720</rowOff>
+      <col>135</col>
+      <colOff>594720</colOff>
+      <row>34</row>
+      <rowOff>11880</rowOff>
     </to>
     <graphicFrame>
       <nvGraphicFramePr>
@@ -797,635 +770,392 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.66796875" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
-  <cols>
-    <col width="16.2" customWidth="1" style="8" min="6" max="6"/>
-    <col width="14.38" customWidth="1" style="9" min="7" max="7"/>
-    <col width="140.36" customWidth="1" style="8" min="10" max="10"/>
-    <col width="13.5" customWidth="1" style="8" min="12" max="12"/>
-    <col width="139.25" customWidth="1" style="8" min="34" max="34"/>
-    <col width="15.61" customWidth="1" style="8" min="35" max="35"/>
-    <col width="15.61" customWidth="1" style="10" min="36" max="36"/>
-    <col width="37.25" customWidth="1" style="8" min="37" max="37"/>
-    <col width="37.25" customWidth="1" style="10" min="39" max="39"/>
-    <col width="11.5" customWidth="1" style="9" min="40" max="40"/>
-    <col width="15.61" customWidth="1" style="10" min="75" max="75"/>
-    <col width="11.5" customWidth="1" style="10" min="76" max="76"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" s="11">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="6">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
-        <is>
-          <t>Adresse de courriel</t>
-        </is>
-      </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Réponse 1</t>
         </is>
       </c>
-      <c r="G1" s="12" t="inlineStr">
-        <is>
-          <t>Les chromosomes du père déterminent si le bébé est un garçon ou une fille</t>
-        </is>
-      </c>
-      <c r="H1" s="12" t="inlineStr">
-        <is>
-          <t>accuracy_Q1</t>
-        </is>
-      </c>
-      <c r="I1" s="12" t="inlineStr">
-        <is>
-          <t>accuracy_Q12</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="11">
-      <c r="A2" s="8" t="inlineStr">
+    </row>
+    <row r="2" ht="12.75" customHeight="1" s="6">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="B2" s="8" t="inlineStr">
-        <is>
-          <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C2" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D2" s="13" t="inlineStr">
-        <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="F2" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G2" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1" s="11">
-      <c r="A3" s="8" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.75" customHeight="1" s="6">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
-        <is>
-          <t>zina.abbas@universite-paris-saclay.fr</t>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C3" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D3" s="13" t="inlineStr">
-        <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="D3" s="7" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G3" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1" s="11">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1" s="6">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="B4" s="8" t="inlineStr">
-        <is>
-          <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C4" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>7,98</t>
         </is>
       </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G4" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" s="11">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="E4" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1" s="6">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D5" s="13" t="inlineStr">
-        <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="D5" s="7" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="F5" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G5" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Faux</t>
-        </is>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1" s="11">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.75" customHeight="1" s="6">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="B6" s="8" t="inlineStr">
-        <is>
-          <t>yasmine.abdelali@universite-paris-saclay.fr</t>
+      <c r="B6" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C6" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D6" s="13" t="inlineStr">
-        <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="D6" s="7" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="F6" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1" s="11">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="E6" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.75" customHeight="1" s="6">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
-        <is>
-          <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D7" s="14" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="D7" s="7" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="F7" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G7" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Faux</t>
-        </is>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1" s="11">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="E7" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.75" customHeight="1" s="6">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="B8" s="8" t="inlineStr">
-        <is>
-          <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
+      <c r="B8" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C8" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D8" s="13" t="inlineStr">
-        <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="D8" s="7" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="F8" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G8" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1" s="11">
-      <c r="A9" s="8" t="inlineStr">
+      <c r="E8" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.75" customHeight="1" s="6">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="B9" s="8" t="inlineStr">
-        <is>
-          <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
+      <c r="B9" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C9" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D9" s="13" t="inlineStr">
-        <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="D9" s="7" t="inlineStr">
         <is>
           <t>8,07</t>
         </is>
       </c>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G9" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Faux</t>
-        </is>
-      </c>
-      <c r="H9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" s="11">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="E9" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.75" customHeight="1" s="6">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="B10" s="8" t="inlineStr">
-        <is>
-          <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
+      <c r="B10" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C10" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D10" s="13" t="inlineStr">
-        <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="D10" s="7" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="F10" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G10" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1" s="11">
-      <c r="A11" s="8" t="inlineStr">
+      <c r="E10" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="12.75" customHeight="1" s="6">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="B11" s="8" t="inlineStr">
-        <is>
-          <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
+      <c r="B11" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D11" s="13" t="inlineStr">
-        <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="D11" s="7" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G11" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Je ne sais pas</t>
-        </is>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" s="11">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="12.75" customHeight="1" s="6">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="B12" s="8" t="inlineStr">
-        <is>
-          <t>20221641@etud.univ-evry.fr</t>
+      <c r="B12" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C12" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D12" s="13" t="inlineStr">
-        <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="D12" s="7" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="F12" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G12" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Faux</t>
-        </is>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" s="11">
-      <c r="A13" s="15" t="inlineStr">
+      <c r="E12" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="12.75" customHeight="1" s="6">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="B13" s="8" t="inlineStr">
-        <is>
-          <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
+      <c r="B13" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
         </is>
       </c>
       <c r="C13" s="8" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D13" s="13" t="inlineStr">
-        <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="D13" s="7" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G13" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Vrai</t>
-        </is>
-      </c>
-      <c r="H13" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" s="11">
-      <c r="A14" s="15" t="inlineStr">
+      <c r="E13" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="12.75" customHeight="1" s="6">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="B14" s="8" t="inlineStr">
-        <is>
-          <t>christian.abi-rizk@universite-paris-saclay.fr</t>
-        </is>
-      </c>
-      <c r="C14" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr">
+      <c r="B14" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="C14" s="9" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="D14" s="7" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="F14" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G14" s="8" t="inlineStr">
-        <is>
-          <t>partie 1 : Faux</t>
-        </is>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="1048576" ht="12.75" customHeight="1" s="11"/>
+      <c r="E14" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.3" right="0.3" top="0.6097222222222221" bottom="0.370138888888889" header="0.1" footer="0.1"/>
@@ -1450,683 +1180,683 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="11">
-      <c r="A1" s="8" t="inlineStr">
+    <row r="1" ht="12.75" customHeight="1" s="6">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Prénom</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
         <is>
           <t>Adresse de courriel</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="7" t="inlineStr">
         <is>
           <t>État</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="7" t="inlineStr">
         <is>
           <t>Temps utilisé</t>
         </is>
       </c>
-      <c r="E1" s="8" t="inlineStr">
+      <c r="E1" s="7" t="inlineStr">
         <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="F1" s="8" t="inlineStr">
+      <c r="F1" s="7" t="inlineStr">
         <is>
           <t>Réponse 1</t>
         </is>
       </c>
-      <c r="G1" s="12" t="inlineStr">
+      <c r="G1" s="11" t="inlineStr">
         <is>
           <t>Les chromosomes du père déterminent si le bébé est un garçon ou une fille</t>
         </is>
       </c>
-      <c r="H1" s="12" t="inlineStr">
+      <c r="H1" s="11" t="inlineStr">
         <is>
           <t>accuracy_Q1</t>
         </is>
       </c>
-      <c r="I1" s="12" t="inlineStr">
+      <c r="I1" s="11" t="inlineStr">
         <is>
           <t>accuracy_Q12</t>
         </is>
       </c>
-      <c r="J1" s="12" t="inlineStr">
+      <c r="J1" s="11" t="inlineStr">
         <is>
           <t xml:space="preserve">Le centre de la Terre est très chaud </t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.75" customHeight="1" s="11">
-      <c r="A2" s="8" t="inlineStr">
+    <row r="2" ht="12.75" customHeight="1" s="6">
+      <c r="A2" s="7" t="inlineStr">
         <is>
           <t>Paola</t>
         </is>
       </c>
-      <c r="B2" s="8" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>paola.aatif-mieulet@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C2" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D2" s="13" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
         <is>
           <t>8 min 33 s</t>
         </is>
       </c>
-      <c r="E2" s="8" t="inlineStr">
+      <c r="E2" s="7" t="inlineStr">
         <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="F2" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G2" s="8" t="inlineStr">
+      <c r="F2" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G2" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H2" s="8" t="n">
+      <c r="H2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I2" s="8" t="n">
+      <c r="I2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J2" s="8" t="inlineStr">
+      <c r="J2" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1" s="11">
-      <c r="A3" s="8" t="inlineStr">
+    <row r="3" ht="12.75" customHeight="1" s="6">
+      <c r="A3" s="7" t="inlineStr">
         <is>
           <t>Zina</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>zina.abbas@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C3" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D3" s="13" t="inlineStr">
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
         <is>
           <t>5 min 15 s</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="7" t="inlineStr">
         <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="F3" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G3" s="8" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G3" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="8" t="n">
+      <c r="I3" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="8" t="inlineStr">
+      <c r="J3" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.75" customHeight="1" s="11">
-      <c r="A4" s="8" t="inlineStr">
+    <row r="4" ht="12.75" customHeight="1" s="6">
+      <c r="A4" s="7" t="inlineStr">
         <is>
           <t>Aboubaker</t>
         </is>
       </c>
-      <c r="B4" s="8" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>aboubaker.abdallah@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C4" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr">
+      <c r="C4" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
         <is>
           <t>7 min 57 s</t>
         </is>
       </c>
-      <c r="E4" s="8" t="inlineStr">
+      <c r="E4" s="7" t="inlineStr">
         <is>
           <t>7,98</t>
         </is>
       </c>
-      <c r="F4" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G4" s="8" t="inlineStr">
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G4" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="I4" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J4" s="8" t="inlineStr">
+      <c r="J4" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="12.75" customHeight="1" s="11">
-      <c r="A5" s="8" t="inlineStr">
+    <row r="5" ht="12.75" customHeight="1" s="6">
+      <c r="A5" s="7" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>yasmine.abdel-moneim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C5" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D5" s="13" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>7 min 22 s</t>
         </is>
       </c>
-      <c r="E5" s="8" t="inlineStr">
+      <c r="E5" s="7" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="F5" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G5" s="8" t="inlineStr">
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G5" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Faux</t>
         </is>
       </c>
-      <c r="H5" s="8" t="n">
+      <c r="H5" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="I5" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="8" t="inlineStr">
+      <c r="J5" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="12.75" customHeight="1" s="11">
-      <c r="A6" s="8" t="inlineStr">
+    <row r="6" ht="12.75" customHeight="1" s="6">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>Yasmine</t>
         </is>
       </c>
-      <c r="B6" s="8" t="inlineStr">
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>yasmine.abdelali@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C6" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D6" s="13" t="inlineStr">
+      <c r="C6" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D6" s="8" t="inlineStr">
         <is>
           <t>7 min 44 s</t>
         </is>
       </c>
-      <c r="E6" s="8" t="inlineStr">
+      <c r="E6" s="7" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="F6" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G6" s="8" t="inlineStr">
+      <c r="F6" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G6" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="H6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="I6" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J6" s="8" t="inlineStr">
+      <c r="J6" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="12.75" customHeight="1" s="11">
-      <c r="A7" s="8" t="inlineStr">
+    <row r="7" ht="12.75" customHeight="1" s="6">
+      <c r="A7" s="7" t="inlineStr">
         <is>
           <t>Hassan Mahamat</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
+      <c r="B7" s="7" t="inlineStr">
         <is>
           <t>hassan-mahamat.abdelgow@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C7" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D7" s="14" t="inlineStr">
+      <c r="C7" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
         <is>
           <t>23 min 37 s</t>
         </is>
       </c>
-      <c r="E7" s="8" t="inlineStr">
+      <c r="E7" s="7" t="inlineStr">
         <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="F7" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G7" s="8" t="inlineStr">
+      <c r="F7" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G7" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Faux</t>
         </is>
       </c>
-      <c r="H7" s="8" t="n">
+      <c r="H7" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="8" t="n">
+      <c r="I7" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="J7" s="8" t="inlineStr">
+      <c r="J7" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.75" customHeight="1" s="11">
-      <c r="A8" s="8" t="inlineStr">
+    <row r="8" ht="12.75" customHeight="1" s="6">
+      <c r="A8" s="7" t="inlineStr">
         <is>
           <t>Nouh</t>
         </is>
       </c>
-      <c r="B8" s="8" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>nouh.abdelhadi@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D8" s="13" t="inlineStr">
+      <c r="C8" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>9 min 27 s</t>
         </is>
       </c>
-      <c r="E8" s="8" t="inlineStr">
+      <c r="E8" s="7" t="inlineStr">
         <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="F8" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G8" s="8" t="inlineStr">
+      <c r="F8" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G8" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H8" s="8" t="n">
+      <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="8" t="n">
+      <c r="I8" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J8" s="8" t="inlineStr">
+      <c r="J8" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="12.75" customHeight="1" s="11">
-      <c r="A9" s="8" t="inlineStr">
+    <row r="9" ht="12.75" customHeight="1" s="6">
+      <c r="A9" s="7" t="inlineStr">
         <is>
           <t>Yacine</t>
         </is>
       </c>
-      <c r="B9" s="8" t="inlineStr">
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>yacine.abdelkarim@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D9" s="13" t="inlineStr">
+      <c r="C9" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D9" s="8" t="inlineStr">
         <is>
           <t>4 min 17 s</t>
         </is>
       </c>
-      <c r="E9" s="8" t="inlineStr">
+      <c r="E9" s="7" t="inlineStr">
         <is>
           <t>8,07</t>
         </is>
       </c>
-      <c r="F9" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G9" s="8" t="inlineStr">
+      <c r="F9" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G9" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Faux</t>
         </is>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="I9" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="8" t="inlineStr">
+      <c r="J9" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="12.75" customHeight="1" s="11">
-      <c r="A10" s="8" t="inlineStr">
+    <row r="10" ht="12.75" customHeight="1" s="6">
+      <c r="A10" s="7" t="inlineStr">
         <is>
           <t>Iness</t>
         </is>
       </c>
-      <c r="B10" s="8" t="inlineStr">
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>iness.abdenbaoui@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C10" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D10" s="13" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D10" s="8" t="inlineStr">
         <is>
           <t>10 min 33 s</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="7" t="inlineStr">
         <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="F10" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G10" s="8" t="inlineStr">
+      <c r="F10" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G10" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H10" s="8" t="n">
+      <c r="H10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="8" t="n">
+      <c r="I10" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J10" s="8" t="inlineStr">
+      <c r="J10" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="12.75" customHeight="1" s="11">
-      <c r="A11" s="8" t="inlineStr">
+    <row r="11" ht="12.75" customHeight="1" s="6">
+      <c r="A11" s="7" t="inlineStr">
         <is>
           <t>Houzefa</t>
         </is>
       </c>
-      <c r="B11" s="8" t="inlineStr">
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>houzefa.abdulhoussen@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D11" s="13" t="inlineStr">
+      <c r="C11" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D11" s="8" t="inlineStr">
         <is>
           <t>5 min 49 s</t>
         </is>
       </c>
-      <c r="E11" s="8" t="inlineStr">
+      <c r="E11" s="7" t="inlineStr">
         <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="F11" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G11" s="8" t="inlineStr">
+      <c r="F11" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G11" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Je ne sais pas</t>
         </is>
       </c>
-      <c r="H11" s="8" t="n">
+      <c r="H11" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I11" s="8" t="n">
+      <c r="I11" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J11" s="8" t="inlineStr">
+      <c r="J11" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="12.75" customHeight="1" s="11">
-      <c r="A12" s="8" t="inlineStr">
+    <row r="12" ht="12.75" customHeight="1" s="6">
+      <c r="A12" s="7" t="inlineStr">
         <is>
           <t>Zakaria</t>
         </is>
       </c>
-      <c r="B12" s="8" t="inlineStr">
+      <c r="B12" s="7" t="inlineStr">
         <is>
           <t>20221641@etud.univ-evry.fr</t>
         </is>
       </c>
-      <c r="C12" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D12" s="13" t="inlineStr">
+      <c r="C12" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D12" s="8" t="inlineStr">
         <is>
           <t>9 min 14 s</t>
         </is>
       </c>
-      <c r="E12" s="8" t="inlineStr">
+      <c r="E12" s="7" t="inlineStr">
         <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="F12" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G12" s="8" t="inlineStr">
+      <c r="F12" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G12" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Faux</t>
         </is>
       </c>
-      <c r="H12" s="8" t="n">
+      <c r="H12" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I12" s="8" t="n">
+      <c r="I12" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J12" s="8" t="inlineStr">
+      <c r="J12" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="12.75" customHeight="1" s="11">
-      <c r="A13" s="15" t="inlineStr">
+    <row r="13" ht="12.75" customHeight="1" s="6">
+      <c r="A13" s="10" t="inlineStr">
         <is>
           <t>Rodolphe</t>
         </is>
       </c>
-      <c r="B13" s="8" t="inlineStr">
+      <c r="B13" s="7" t="inlineStr">
         <is>
           <t>rodolphe.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C13" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D13" s="13" t="inlineStr">
+      <c r="C13" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D13" s="8" t="inlineStr">
         <is>
           <t>15 min 32 s</t>
         </is>
       </c>
-      <c r="E13" s="8" t="inlineStr">
+      <c r="E13" s="7" t="inlineStr">
         <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="F13" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G13" s="8" t="inlineStr">
+      <c r="F13" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G13" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Vrai</t>
         </is>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H13" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="I13" s="8" t="n">
+      <c r="I13" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J13" s="8" t="inlineStr">
+      <c r="J13" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="12.75" customHeight="1" s="11">
-      <c r="A14" s="15" t="inlineStr">
+    <row r="14" ht="12.75" customHeight="1" s="6">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>Christian</t>
         </is>
       </c>
-      <c r="B14" s="8" t="inlineStr">
+      <c r="B14" s="7" t="inlineStr">
         <is>
           <t>christian.abi-rizk@universite-paris-saclay.fr</t>
         </is>
       </c>
-      <c r="C14" s="8" t="inlineStr">
-        <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="D14" s="14" t="inlineStr">
+      <c r="C14" s="7" t="inlineStr">
+        <is>
+          <t>Terminé</t>
+        </is>
+      </c>
+      <c r="D14" s="9" t="inlineStr">
         <is>
           <t>21 min 49 s</t>
         </is>
       </c>
-      <c r="E14" s="8" t="inlineStr">
+      <c r="E14" s="7" t="inlineStr">
         <is>
           <t>6,72</t>
         </is>
       </c>
-      <c r="F14" s="8" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
-      <c r="G14" s="8" t="inlineStr">
+      <c r="F14" s="7" t="inlineStr">
+        <is>
+          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
+        </is>
+      </c>
+      <c r="G14" s="7" t="inlineStr">
         <is>
           <t>partie 1 : Faux</t>
         </is>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="H14" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="I14" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="J14" s="8" t="inlineStr">
+      <c r="J14" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve"> partie 13 : Vrai</t>
         </is>

</xml_diff>